<commit_message>
delete course_student, image atten show
</commit_message>
<xml_diff>
--- a/excel_tmp.xlsx
+++ b/excel_tmp.xlsx
@@ -20,24 +20,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA9067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Anh Tu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA9044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khiem</t>
+    <t xml:space="preserve">last</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA9-060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vũ Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thư</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMSN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThuVM.ba9060@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA9-074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Võ Ngân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thảo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThaoVN.ba9074@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI10-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnhNM.BI10-004@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI10-011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đỗ Thái </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnhDT.BI10-011@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI10-102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Diệu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinhND.BI10-102@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI10-151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng Minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QuanHM.BI10-151@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI10-190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Gia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viễn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VienNG.BI10-190@st.usth.edu.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA9-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hồ Thị Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đào</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DaoHTA.ba9013@st.usth.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -47,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -68,6 +167,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +222,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -138,13 +243,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.48"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -153,21 +261,177 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>